<commit_message>
used mapping_file creator, worked on qubit_on_cfx analyzer
used the mapping_file creator on Sofia Ledin's lane. NOTE: make sure that the file, primer names etc is in the correct format!

qubit_on_cfx works. but I want to make it look nicer and save the results in a file. maybe do it in jupyter?
</commit_message>
<xml_diff>
--- a/mapping_file_creator/user_template_for_mappingfile_creatorpy.xlsx
+++ b/mapping_file_creator/user_template_for_mappingfile_creatorpy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ZEUS\mmb\molecular_ecology\mollab_team\Sequencing\ngs_sequencing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrouwer\Documents\molecular_tools\mapping_file_creator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A664ED5-9DAD-4E3B-9026-80DA254BF454}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF6A13A-4B76-495B-8E49-D4D4AED057CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7070" xr2:uid="{68034F01-8106-4319-987A-44FA225DB157}"/>
+    <workbookView xWindow="-28920" yWindow="-495" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{68034F01-8106-4319-987A-44FA225DB157}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1575,19 +1575,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A57F65-611E-42F6-A955-ACF7D10AD9DD}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1624,676 +1624,676 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A5BD60-D995-420A-BB61-B31683758674}">
   <dimension ref="A1:A133"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>139</v>
       </c>
@@ -2311,672 +2311,672 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>270</v>
       </c>
@@ -2994,652 +2994,652 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>397</v>
       </c>

</xml_diff>

<commit_message>
primer xlsx file instead of seperate csvs
</commit_message>
<xml_diff>
--- a/mapping_file_creator/user_template_for_mappingfile_creatorpy.xlsx
+++ b/mapping_file_creator/user_template_for_mappingfile_creatorpy.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrouwer\Documents\molecular_tools\mapping_file_creator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\zeus.nioz.nl\mmb\molecular_ecology\mollab_team\Sequencing\ngs_sequencing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015F59E1-A5AF-446C-A352-D2EF6F9C08FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E087E38-7737-4F81-ADFD-666FC2F047FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="-120" windowWidth="24330" windowHeight="15990" xr2:uid="{68034F01-8106-4319-987A-44FA225DB157}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E87429A6-9664-4425-8D48-E5D0FCAA54B2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="515F" sheetId="2" r:id="rId2"/>
-    <sheet name="806RB" sheetId="3" r:id="rId3"/>
-    <sheet name="926RBC" sheetId="4" r:id="rId4"/>
-    <sheet name="12S_F1a" sheetId="5" r:id="rId5"/>
-    <sheet name="12S_R1" sheetId="6" r:id="rId6"/>
+    <sheet name="HowToUse" sheetId="7" r:id="rId1"/>
+    <sheet name="ReadMe" sheetId="8" r:id="rId2"/>
+    <sheet name="FILL_IN" sheetId="1" r:id="rId3"/>
+    <sheet name="515F" sheetId="2" r:id="rId4"/>
+    <sheet name="806RB" sheetId="3" r:id="rId5"/>
+    <sheet name="926RBC" sheetId="4" r:id="rId6"/>
+    <sheet name="12S_F1a" sheetId="5" r:id="rId7"/>
+    <sheet name="12S_R1" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="513">
   <si>
     <t>Forward_primer</t>
   </si>
@@ -47,9 +49,6 @@
     <t>926RBC_Golay002</t>
   </si>
   <si>
-    <t>Whatever data you want to be close to your results</t>
-  </si>
-  <si>
     <t xml:space="preserve">can be as many columns as you like </t>
   </si>
   <si>
@@ -1497,14 +1496,97 @@
   </si>
   <si>
     <t>12S_R1_Golay084</t>
+  </si>
+  <si>
+    <t>Project_Name</t>
+  </si>
+  <si>
+    <t>NIOZ_Number</t>
+  </si>
+  <si>
+    <t>Forward_Primer</t>
+  </si>
+  <si>
+    <t>Reverse_Primer</t>
+  </si>
+  <si>
+    <t>Project_info</t>
+  </si>
+  <si>
+    <t>Sampling_info</t>
+  </si>
+  <si>
+    <t>Cruise_Number</t>
+  </si>
+  <si>
+    <t>Who_Sampled</t>
+  </si>
+  <si>
+    <t>extraction_method</t>
+  </si>
+  <si>
+    <t>PCR_info</t>
+  </si>
+  <si>
+    <t>Extraction_info</t>
+  </si>
+  <si>
+    <t>polymerase</t>
+  </si>
+  <si>
+    <t>Pool_info</t>
+  </si>
+  <si>
+    <t>quantification_method</t>
+  </si>
+  <si>
+    <t>pooling_methods</t>
+  </si>
+  <si>
+    <t>Sequencing_info</t>
+  </si>
+  <si>
+    <t>sequencing_platform</t>
+  </si>
+  <si>
+    <t>run_type</t>
+  </si>
+  <si>
+    <t>library_prep</t>
+  </si>
+  <si>
+    <t>gel_photos</t>
+  </si>
+  <si>
+    <t>Who_extracted</t>
+  </si>
+  <si>
+    <t>Who_PCRed</t>
+  </si>
+  <si>
+    <t>Who_Poooled</t>
+  </si>
+  <si>
+    <t>Sequencing_company</t>
+  </si>
+  <si>
+    <t>Whatever meta_data differs between your samples</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1532,8 +1614,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1549,6 +1633,734 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2282901-A02E-435B-8595-80C0A2AC1489}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="209550"/>
+          <a:ext cx="7343775" cy="6219825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="1"/>
+            <a:t>How</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="1" baseline="0"/>
+            <a:t> to use this template</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>On the ReadMe sheet write down info that applies to all samples in this sequencing run.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>This can entail:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Project info </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(Project name, number, who is involved and who did what)</a:t>
+          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100" b="1" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>sampling info </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(Cruise number, whatever else is the same for all samples) </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>extraction info </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(method, etc)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>PCR info </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(polymerase, primers, etc.)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>pool info</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> (quantification method, pooling method)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>sequencing info </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(platform, run_type, library_prep)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-NL">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>In the FILL</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t> IN sheet enter info that differs among the samples.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>Columns $1 and $2 must contain the forward and reverse primer barcode numbers. These need to be in the exact format as on the following primer sheets.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="nl-NL" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>After the 2 primer columns, there can be as many columns as you want with sample data. This should be data that differs between samples. This can entail:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>sampling info </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(sample_type, date, depth, coordinates, CTD measurements etc.) </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-NL">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>extraction info </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(method, concentration, nanodrop info etc)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-NL">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>PCR info </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(visible bands (also a link to your (labelled) electrophoresis gel photo's would be nice to have))</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-NL">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>pool info</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> (amplicon concentration, pooled amount, etc.)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-NL">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="nl-NL" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>The last column always needs to be the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="1" baseline="0"/>
+            <a:t>description </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="0" baseline="0"/>
+            <a:t>of your samples</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>. This can be a sample code or name. However you call your sample, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="1" u="sng" baseline="0"/>
+            <a:t>do not use spaces or weird signs</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>. Only _ or - and . can be used.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>Anything after the description column will not be included in the mapping file.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>In the description column, mark positive and negative controls clearly.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>They should contain the following abbreviations </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>sampling negative =  Neg_samp</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>extraction negative = Neg_extr</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>PCR negative =  Neg_PCR</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Mock community Zymo DNA log = Mock_Zdna-D6311</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Mock community Zymo cells = Mock_Zcell-D6331</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Mock community custom DNA = Mock_cust</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1847,18 +2659,170 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2D820C-9245-4BF5-B192-98C8BE280062}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1E1336-1800-4209-967A-86A8597EDD7B}">
+  <dimension ref="A1:A29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>506</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A57F65-611E-42F6-A955-ACF7D10AD9DD}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="109.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1870,10 +2834,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>512</v>
       </c>
       <c r="D1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1884,45 +2848,45 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>
@@ -1930,7 +2894,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A5BD60-D995-420A-BB61-B31683758674}">
   <dimension ref="A1:A133"/>
   <sheetViews>
@@ -1953,657 +2917,657 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2611,13 +3575,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F064B2-3790-47E0-8AD5-AC356B6E79ED}">
   <dimension ref="A1:A133"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2636,657 +3598,657 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -3294,7 +4256,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A6BC35A-26B3-43D2-829C-9D02DA88928F}">
   <dimension ref="A1:A129"/>
   <sheetViews>
@@ -3317,637 +4279,637 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -3955,13 +4917,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4243F361-F3AE-4CB8-B4C8-9C518B07F300}">
   <dimension ref="A1:A43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3975,212 +4935,212 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -4188,13 +5148,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5BD161C-0978-4F9D-938B-50EDD805F94A}">
   <dimension ref="A1:A43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A43"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4205,212 +5163,212 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
primers with 3 or 4 digits
working on it... does not work yet with 4 digits
</commit_message>
<xml_diff>
--- a/mapping_file_creator/user_template_for_mappingfile_creatorpy.xlsx
+++ b/mapping_file_creator/user_template_for_mappingfile_creatorpy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\zeus.nioz.nl\mmb\molecular_ecology\mollab_team\Sequencing\ngs_sequencing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://joinnioz-my.sharepoint.com/personal/maartje_brouwer_nioz_nl/Documents/Documenten/GitHub/molecular_tools/mapping_file_creator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936A02D3-5C77-4F24-8021-037AB118700B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{936A02D3-5C77-4F24-8021-037AB118700B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA05A907-137B-46C9-B157-FAB1A9D736DE}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{E87429A6-9664-4425-8D48-E5D0FCAA54B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E87429A6-9664-4425-8D48-E5D0FCAA54B2}"/>
   </bookViews>
   <sheets>
     <sheet name="HowToUse" sheetId="7" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="144">
   <si>
     <t>Forward_primer</t>
   </si>
@@ -189,40 +189,301 @@
     <t>V3 kit 2 x 300 bp</t>
   </si>
   <si>
-    <t>FW001</t>
-  </si>
-  <si>
-    <t>RV002</t>
-  </si>
-  <si>
-    <t>FW003</t>
-  </si>
-  <si>
-    <t>RV004</t>
-  </si>
-  <si>
-    <t>RV006</t>
-  </si>
-  <si>
-    <t>FW007</t>
-  </si>
-  <si>
-    <t>RV008</t>
-  </si>
-  <si>
-    <t>FW009</t>
-  </si>
-  <si>
-    <t>RV010</t>
-  </si>
-  <si>
-    <t>FW011</t>
-  </si>
-  <si>
-    <t>RV012</t>
-  </si>
-  <si>
-    <t>FW005</t>
+    <t>515F_Golay0241</t>
+  </si>
+  <si>
+    <t>515F_Golay0243</t>
+  </si>
+  <si>
+    <t>515F_Golay0245</t>
+  </si>
+  <si>
+    <t>515F_Golay0247</t>
+  </si>
+  <si>
+    <t>515F_Golay0249</t>
+  </si>
+  <si>
+    <t>515F_Golay0251</t>
+  </si>
+  <si>
+    <t>515F_Golay0253</t>
+  </si>
+  <si>
+    <t>515F_Golay0255</t>
+  </si>
+  <si>
+    <t>515F_Golay0401</t>
+  </si>
+  <si>
+    <t>515F_Golay0402</t>
+  </si>
+  <si>
+    <t>515F_Golay0403</t>
+  </si>
+  <si>
+    <t>515F_Golay0404</t>
+  </si>
+  <si>
+    <t>515F_Golay9001</t>
+  </si>
+  <si>
+    <t>515F_Golay9003</t>
+  </si>
+  <si>
+    <t>515F_Golay9005</t>
+  </si>
+  <si>
+    <t>515F_Golay9007</t>
+  </si>
+  <si>
+    <t>515F_Golay9009</t>
+  </si>
+  <si>
+    <t>515F_Golay9011</t>
+  </si>
+  <si>
+    <t>515F_Golay9013</t>
+  </si>
+  <si>
+    <t>515F_Golay9015</t>
+  </si>
+  <si>
+    <t>515F_Golay9017</t>
+  </si>
+  <si>
+    <t>515F_Golay9019</t>
+  </si>
+  <si>
+    <t>515F_Golay9021</t>
+  </si>
+  <si>
+    <t>515F_Golay9023</t>
+  </si>
+  <si>
+    <t>515F_Golay9025</t>
+  </si>
+  <si>
+    <t>515F_Golay9027</t>
+  </si>
+  <si>
+    <t>515F_Golay9029</t>
+  </si>
+  <si>
+    <t>515F_Golay9031</t>
+  </si>
+  <si>
+    <t>515F_Golay9033</t>
+  </si>
+  <si>
+    <t>515F_Golay9035</t>
+  </si>
+  <si>
+    <t>515F_Golay9037</t>
+  </si>
+  <si>
+    <t>515F_Golay9039</t>
+  </si>
+  <si>
+    <t>515F_Golay9041</t>
+  </si>
+  <si>
+    <t>926RBC_Golay0160</t>
+  </si>
+  <si>
+    <t>926RBC_Golay0162</t>
+  </si>
+  <si>
+    <t>926RBC_Golay0164</t>
+  </si>
+  <si>
+    <t>926RBC_Golay0166</t>
+  </si>
+  <si>
+    <t>926RBC_Golay0168</t>
+  </si>
+  <si>
+    <t>926RBC_Golay0170</t>
+  </si>
+  <si>
+    <t>926RBC_Golay9046</t>
+  </si>
+  <si>
+    <t>926RBC_Golay9048</t>
+  </si>
+  <si>
+    <t>926RBC_Golay9050</t>
+  </si>
+  <si>
+    <t>926RBC_Golay9052</t>
+  </si>
+  <si>
+    <t>926RBC_Golay9054</t>
+  </si>
+  <si>
+    <t>926RBC_Golay9056</t>
+  </si>
+  <si>
+    <t>926RBC_Golay9058</t>
+  </si>
+  <si>
+    <t>926RBC_Golay9060</t>
+  </si>
+  <si>
+    <t>926RBC_Golay9062</t>
+  </si>
+  <si>
+    <t>926RBC_Golay9064</t>
+  </si>
+  <si>
+    <t>926RBC_Golay0024</t>
+  </si>
+  <si>
+    <t>926RBC_Golay0026</t>
+  </si>
+  <si>
+    <t>926RBC_Golay0028</t>
+  </si>
+  <si>
+    <t>926RBC_Golay0030</t>
+  </si>
+  <si>
+    <t>926RBC_Golay0032</t>
+  </si>
+  <si>
+    <t>926RBC_Golay0034</t>
+  </si>
+  <si>
+    <t>926RBC_Golay0036</t>
+  </si>
+  <si>
+    <t>926RBC_Golay9106</t>
+  </si>
+  <si>
+    <t>926RBC_Golay9108</t>
+  </si>
+  <si>
+    <t>926RBC_Golay9110</t>
+  </si>
+  <si>
+    <t>926RBC_Golay9112</t>
+  </si>
+  <si>
+    <t>926RBC_Golay9114</t>
+  </si>
+  <si>
+    <t>926RBC_Golay9116</t>
+  </si>
+  <si>
+    <t>926RBC_Golay9118</t>
+  </si>
+  <si>
+    <t>926RBC_Golay9120</t>
+  </si>
+  <si>
+    <t>926RBC_Golay9122</t>
+  </si>
+  <si>
+    <t>926RBC_Golay9124</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
+    <t>S11</t>
+  </si>
+  <si>
+    <t>S12</t>
+  </si>
+  <si>
+    <t>S13</t>
+  </si>
+  <si>
+    <t>S14</t>
+  </si>
+  <si>
+    <t>S15</t>
+  </si>
+  <si>
+    <t>S16</t>
+  </si>
+  <si>
+    <t>S17</t>
+  </si>
+  <si>
+    <t>S18</t>
+  </si>
+  <si>
+    <t>S19</t>
+  </si>
+  <si>
+    <t>S20</t>
+  </si>
+  <si>
+    <t>S21</t>
+  </si>
+  <si>
+    <t>S22</t>
+  </si>
+  <si>
+    <t>S23</t>
+  </si>
+  <si>
+    <t>S24</t>
+  </si>
+  <si>
+    <t>S25</t>
+  </si>
+  <si>
+    <t>S26</t>
+  </si>
+  <si>
+    <t>S27</t>
+  </si>
+  <si>
+    <t>S28</t>
+  </si>
+  <si>
+    <t>S29</t>
+  </si>
+  <si>
+    <t>S30</t>
+  </si>
+  <si>
+    <t>S31</t>
+  </si>
+  <si>
+    <t>S32</t>
+  </si>
+  <si>
+    <t>S33</t>
   </si>
 </sst>
 </file>
@@ -1683,10 +1944,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A57F65-611E-42F6-A955-ACF7D10AD9DD}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1713,52 +1974,379 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="B13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38"/>
     </row>
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>

</xml_diff>